<commit_message>
Support for Closed.Xml 0.95.0
</commit_message>
<xml_diff>
--- a/ExcelReportGenerator.Tests/TestData/DataSourceDynamicPanelDataSetRenderTest/TestRenderDataSetWithEvents_HorizontalPanel.xlsx
+++ b/ExcelReportGenerator.Tests/TestData/DataSourceDynamicPanelDataSetRenderTest/TestRenderDataSetWithEvents_HorizontalPanel.xlsx
@@ -111,7 +111,6 @@
     <x:fill>
       <x:patternFill patternType="solid">
         <x:fgColor rgb="FF00DDDD"/>
-        <x:bgColor rgb="FF00DDDD"/>
       </x:patternFill>
     </x:fill>
   </x:fills>
@@ -281,10 +280,10 @@
     <x:xf numFmtId="0" fontId="1" fillId="0" borderId="6" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="167" fontId="2" fillId="2" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
     <x:xf numFmtId="167" fontId="3" fillId="0" borderId="7" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="167" fontId="2" fillId="2" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
@@ -325,11 +324,11 @@
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="167" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
     <x:xf numFmtId="167" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="167" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -689,9 +688,7 @@
       <x:c r="D5" s="2" t="n">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="E5" s="2" t="n">
-        <x:v>1</x:v>
-      </x:c>
+      <x:c r="E5" s="2" t="s"/>
       <x:c r="F5" s="5" t="s"/>
     </x:row>
     <x:row r="6" spans="1:6">
@@ -726,16 +723,16 @@
       <x:c r="B8" s="8" t="s">
         <x:v>13</x:v>
       </x:c>
-      <x:c r="C8" s="10" t="n">
+      <x:c r="C8" s="9" t="n">
         <x:v>2.6</x:v>
       </x:c>
-      <x:c r="D8" s="10" t="n">
+      <x:c r="D8" s="9" t="n">
         <x:v>5.2</x:v>
       </x:c>
-      <x:c r="E8" s="10" t="n">
+      <x:c r="E8" s="9" t="n">
         <x:v>7.8</x:v>
       </x:c>
-      <x:c r="F8" s="9" t="n">
+      <x:c r="F8" s="10" t="n">
         <x:v>15.6</x:v>
       </x:c>
     </x:row>

</xml_diff>